<commit_message>
Agregado a precondicion:"Que existan campañas vigentes." Cambiado numero de version
</commit_message>
<xml_diff>
--- a/CU1.3 Ver Campaña.xlsx
+++ b/CU1.3 Ver Campaña.xlsx
@@ -73,16 +73,17 @@
     <t>Caso de Uso</t>
   </si>
   <si>
-    <t>0001</t>
-  </si>
-  <si>
     <t>El sistema busca en la base de datos todos los datos coincidentes con el id de la campaña seleccionada y los presenta en pantalla a través del formulario Campaña.</t>
   </si>
   <si>
-    <t>Que el actor tenga los permisos necesarios para ver el registro.</t>
-  </si>
-  <si>
     <t>El actor hace clic en el botón "Ver" en algún registro de listado de campañas</t>
+  </si>
+  <si>
+    <t>Que el actor tenga los permisos necesarios para ver el registro.
+Que existan campañas vigentes.</t>
+  </si>
+  <si>
+    <t>0002</t>
   </si>
 </sst>
 </file>
@@ -544,7 +545,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +594,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C5" s="7"/>
     </row>
@@ -624,7 +625,7 @@
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -652,7 +653,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C12" s="10"/>
     </row>
@@ -661,7 +662,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="10"/>
     </row>

</xml_diff>

<commit_message>
Modificacion de descripcion, puntos de extension y curso básico
</commit_message>
<xml_diff>
--- a/CU1.3 Ver Campaña.xlsx
+++ b/CU1.3 Ver Campaña.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Se completaron todos los registros del formulario Campaña.</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Actores</t>
   </si>
   <si>
-    <t>Se muestran en pantalla todos los datos de la campaña seleccionada.</t>
-  </si>
-  <si>
     <t>Descripción</t>
   </si>
   <si>
@@ -74,16 +71,58 @@
   </si>
   <si>
     <t>El sistema busca en la base de datos todos los datos coincidentes con el id de la campaña seleccionada y los presenta en pantalla a través del formulario Campaña.</t>
-  </si>
-  <si>
-    <t>El actor hace clic en el botón "Ver" en algún registro de listado de campañas</t>
-  </si>
-  <si>
-    <t>0002</t>
   </si>
   <si>
     <t>Que el actor tenga los permisos necesarios para ver el registro.
 Que existan campañas activas.</t>
+  </si>
+  <si>
+    <t>Se muestran en pantalla todos los datos de la campaña seleccionada incluyendo el botón "Volver".</t>
+  </si>
+  <si>
+    <t>El actor hace click en el botón "Volver"</t>
+  </si>
+  <si>
+    <t>El sistema cierra el formulario.</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Condicion:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> El actor quiere ver el detalle de la campaña. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Punto de extensión</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>: Paso 2.c del CU01 Administracion de Supervisores:  El actor hace clic en el botón "Ver" del registro de campaña del formulario "Administración de Supervisores".</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -551,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -567,7 +606,7 @@
     <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="18"/>
       <c r="B1" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" s="16">
         <v>42890</v>
@@ -575,53 +614,53 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" s="14"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -639,7 +678,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -650,56 +689,72 @@
       <c r="B10" s="19"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="12"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>1</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="10"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12"/>
     </row>
     <row r="13" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
+        <v>1</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
         <v>2</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>3</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="10"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="9"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="1"/>
+      <c r="C19" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>